<commit_message>
Final amendments before submission
</commit_message>
<xml_diff>
--- a/Metadata/marker_genes_heatmaps.xlsx
+++ b/Metadata/marker_genes_heatmaps.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominiquepaul/xRobinson Group/02_Protocol/Metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415ED9FA-BB36-7E4C-A636-48AE9F92511B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC770C7-FC0D-E745-8918-AC68B042D959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-7120" windowWidth="25600" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-7120" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fresh only - High level" sheetId="1" r:id="rId1"/>
     <sheet name="Fresh only - subclusters" sheetId="2" r:id="rId2"/>
     <sheet name="Fresh only - Validation" sheetId="3" r:id="rId3"/>
+    <sheet name="Fresh only - subclusters old" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="151">
   <si>
     <t>Group</t>
   </si>
@@ -435,6 +436,57 @@
   </si>
   <si>
     <t>HMOX+ anti-oxidative papillary</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Secretory reticular MFAP5+</t>
+  </si>
+  <si>
+    <t>FBLN1</t>
+  </si>
+  <si>
+    <t>Anti-oxidative papillary HMOX1+</t>
+  </si>
+  <si>
+    <t>SQSTM1</t>
+  </si>
+  <si>
+    <t>Papillary PLCG2+</t>
+  </si>
+  <si>
+    <t>Transitional KRT1/KRT15med</t>
+  </si>
+  <si>
+    <t>TPM22</t>
+  </si>
+  <si>
+    <t>MYH11</t>
+  </si>
+  <si>
+    <t>PDGFRB+ pericytes</t>
+  </si>
+  <si>
+    <t>PDGFRB</t>
+  </si>
+  <si>
+    <t>COL4A1</t>
+  </si>
+  <si>
+    <t>EDNRB</t>
+  </si>
+  <si>
+    <t>CCL22+ dendritic cells</t>
+  </si>
+  <si>
+    <t>ACTA2+ VSMCs</t>
+  </si>
+  <si>
+    <t>Proinflammatory reticular CCL19+</t>
+  </si>
+  <si>
+    <t>RNASE1+ macrophages</t>
   </si>
 </sst>
 </file>
@@ -1543,25 +1595,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D13"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" style="2"/>
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="37.5" customWidth="1"/>
+    <col min="4" max="4" width="80.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>134</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>37</v>
@@ -1569,1196 +1621,1118 @@
       <c r="D1" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>149</v>
+      </c>
+      <c r="E12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="B13">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="B14">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="B15">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>137</v>
+      </c>
+      <c r="E16" t="s">
         <v>46</v>
       </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" t="s">
         <v>47</v>
       </c>
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>137</v>
+      </c>
+      <c r="E18" t="s">
         <v>48</v>
       </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="B18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>4</v>
       </c>
-      <c r="B19" t="s">
-        <v>55</v>
+      <c r="B19">
+        <v>4</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>4</v>
       </c>
-      <c r="B20" t="s">
-        <v>56</v>
+      <c r="B20">
+        <v>4</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+      <c r="E20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4</v>
       </c>
-      <c r="B21" t="s">
-        <v>57</v>
+      <c r="B21">
+        <v>4</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+      <c r="E21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>4</v>
-      </c>
-      <c r="B22" t="s">
-        <v>103</v>
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+      <c r="E22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5</v>
       </c>
-      <c r="B23" t="s">
-        <v>45</v>
+      <c r="B23">
+        <v>5</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+      <c r="E23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>5</v>
       </c>
-      <c r="B24" t="s">
-        <v>58</v>
+      <c r="B24">
+        <v>5</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+      <c r="E24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>5</v>
-      </c>
-      <c r="B25" t="s">
-        <v>104</v>
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
-      <c r="B26" t="s">
-        <v>57</v>
+      <c r="B26">
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="E26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
-      <c r="B27" t="s">
-        <v>59</v>
+      <c r="B27">
+        <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
-      <c r="B28" t="s">
-        <v>60</v>
+      <c r="B28">
+        <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="E28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
-      <c r="B29" t="s">
-        <v>61</v>
+      <c r="B29">
+        <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="E29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
-      <c r="B30" t="s">
-        <v>62</v>
+      <c r="B30">
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="E30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
-        <v>105</v>
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+      <c r="E31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2</v>
       </c>
-      <c r="B32" t="s">
-        <v>63</v>
+      <c r="B32">
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2</v>
       </c>
-      <c r="B33" t="s">
-        <v>64</v>
+      <c r="B33">
+        <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+      <c r="E33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>2</v>
-      </c>
-      <c r="B34" t="s">
-        <v>65</v>
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="E34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>2</v>
-      </c>
-      <c r="B35" t="s">
-        <v>66</v>
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="E35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36">
         <v>4</v>
       </c>
-      <c r="B36" t="s">
-        <v>67</v>
-      </c>
       <c r="C36" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+      <c r="E36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37">
         <v>4</v>
       </c>
-      <c r="B37" t="s">
-        <v>131</v>
-      </c>
       <c r="C37" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+      <c r="E37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38">
         <v>4</v>
       </c>
-      <c r="B38" t="s">
-        <v>68</v>
-      </c>
       <c r="C38" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+      <c r="E38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39">
         <v>4</v>
       </c>
-      <c r="B39" t="s">
-        <v>48</v>
-      </c>
       <c r="C39" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+      <c r="E39" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40">
         <v>4</v>
       </c>
-      <c r="B40" t="s">
-        <v>69</v>
-      </c>
       <c r="C40" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+      <c r="E40" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>4</v>
-      </c>
-      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" t="s">
+        <v>148</v>
+      </c>
+      <c r="E41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" t="s">
+        <v>148</v>
+      </c>
+      <c r="E42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" t="s">
+        <v>148</v>
+      </c>
+      <c r="E43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" t="s">
+        <v>148</v>
+      </c>
+      <c r="E44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" t="s">
+        <v>148</v>
+      </c>
+      <c r="E45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" t="s">
+        <v>143</v>
+      </c>
+      <c r="E46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" t="s">
+        <v>143</v>
+      </c>
+      <c r="E47" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" t="s">
+        <v>143</v>
+      </c>
+      <c r="E48" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" t="s">
+        <v>143</v>
+      </c>
+      <c r="E49" t="s">
         <v>49</v>
       </c>
-      <c r="C41" t="s">
-        <v>129</v>
-      </c>
-      <c r="D41" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>4</v>
-      </c>
-      <c r="B42" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" t="s">
-        <v>129</v>
-      </c>
-      <c r="D42" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>3</v>
-      </c>
-      <c r="B43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C43" t="s">
-        <v>129</v>
-      </c>
-      <c r="D43" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>3</v>
-      </c>
-      <c r="B44" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" t="s">
-        <v>129</v>
-      </c>
-      <c r="D44" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>3</v>
-      </c>
-      <c r="B45" t="s">
-        <v>71</v>
-      </c>
-      <c r="C45" t="s">
-        <v>129</v>
-      </c>
-      <c r="D45" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>3</v>
-      </c>
-      <c r="B46" t="s">
-        <v>72</v>
-      </c>
-      <c r="C46" t="s">
-        <v>129</v>
-      </c>
-      <c r="D46" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s">
-        <v>74</v>
-      </c>
-      <c r="C47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>1</v>
-      </c>
-      <c r="B48" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>1</v>
-      </c>
-      <c r="B49" t="s">
-        <v>106</v>
-      </c>
-      <c r="C49" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2</v>
       </c>
-      <c r="B50" t="s">
-        <v>74</v>
+      <c r="B50">
+        <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D50" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="E50" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2</v>
       </c>
-      <c r="B51" t="s">
-        <v>8</v>
+      <c r="B51">
+        <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D51" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="E51" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>3</v>
-      </c>
-      <c r="B52" t="s">
-        <v>76</v>
+        <v>2</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D52" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="E52" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>3</v>
-      </c>
-      <c r="B53" t="s">
-        <v>77</v>
+        <v>2</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D53" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="E53" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>3</v>
-      </c>
-      <c r="B54" t="s">
-        <v>110</v>
+        <v>2</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D54" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="E54" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>3</v>
-      </c>
-      <c r="B55" t="s">
-        <v>111</v>
+        <v>2</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D55" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="E55" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>3</v>
-      </c>
-      <c r="B56" t="s">
-        <v>112</v>
+        <v>2</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D56" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="E56" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>4</v>
-      </c>
-      <c r="B57" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D57" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+      <c r="E57" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>4</v>
-      </c>
-      <c r="B58" t="s">
-        <v>79</v>
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D58" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+      <c r="E58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>4</v>
-      </c>
-      <c r="B59" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
       </c>
       <c r="C59" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D59" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+      <c r="E59" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>4</v>
-      </c>
-      <c r="B60" t="s">
-        <v>107</v>
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D60" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+      <c r="E60" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>4</v>
-      </c>
-      <c r="B61" t="s">
-        <v>108</v>
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
       </c>
       <c r="C61" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D61" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+      <c r="E61" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>4</v>
-      </c>
-      <c r="B62" t="s">
-        <v>109</v>
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D62" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>1</v>
-      </c>
-      <c r="B63" t="s">
-        <v>27</v>
-      </c>
-      <c r="C63" t="s">
-        <v>25</v>
-      </c>
-      <c r="D63" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>1</v>
-      </c>
-      <c r="B64" t="s">
-        <v>130</v>
-      </c>
-      <c r="C64" t="s">
-        <v>25</v>
-      </c>
-      <c r="D64" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>1</v>
-      </c>
-      <c r="B65" t="s">
-        <v>80</v>
-      </c>
-      <c r="C65" t="s">
-        <v>25</v>
-      </c>
-      <c r="D65" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>1</v>
-      </c>
-      <c r="B66" t="s">
-        <v>63</v>
-      </c>
-      <c r="C66" t="s">
-        <v>25</v>
-      </c>
-      <c r="D66" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>2</v>
-      </c>
-      <c r="B67" t="s">
-        <v>81</v>
-      </c>
-      <c r="C67" t="s">
-        <v>25</v>
-      </c>
-      <c r="D67" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>2</v>
-      </c>
-      <c r="B68" t="s">
-        <v>62</v>
-      </c>
-      <c r="C68" t="s">
-        <v>25</v>
-      </c>
-      <c r="D68" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>2</v>
-      </c>
-      <c r="B69" t="s">
-        <v>82</v>
-      </c>
-      <c r="C69" t="s">
-        <v>25</v>
-      </c>
-      <c r="D69" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>2</v>
-      </c>
-      <c r="B70" t="s">
-        <v>59</v>
-      </c>
-      <c r="C70" t="s">
-        <v>25</v>
-      </c>
-      <c r="D70" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>3</v>
-      </c>
-      <c r="B71" t="s">
-        <v>49</v>
-      </c>
-      <c r="C71" t="s">
-        <v>25</v>
-      </c>
-      <c r="D71" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>3</v>
-      </c>
-      <c r="B72" t="s">
-        <v>84</v>
-      </c>
-      <c r="C72" t="s">
-        <v>25</v>
-      </c>
-      <c r="D72" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>3</v>
-      </c>
-      <c r="B73" t="s">
-        <v>85</v>
-      </c>
-      <c r="C73" t="s">
-        <v>25</v>
-      </c>
-      <c r="D73" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>3</v>
-      </c>
-      <c r="B74" t="s">
-        <v>86</v>
-      </c>
-      <c r="C74" t="s">
-        <v>25</v>
-      </c>
-      <c r="D74" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>2</v>
-      </c>
-      <c r="B75" t="s">
-        <v>87</v>
-      </c>
-      <c r="C75" t="s">
-        <v>14</v>
-      </c>
-      <c r="D75" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>2</v>
-      </c>
-      <c r="B76" t="s">
-        <v>88</v>
-      </c>
-      <c r="C76" t="s">
-        <v>14</v>
-      </c>
-      <c r="D76" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>2</v>
-      </c>
-      <c r="B77" t="s">
-        <v>89</v>
-      </c>
-      <c r="C77" t="s">
-        <v>14</v>
-      </c>
-      <c r="D77" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>2</v>
-      </c>
-      <c r="B78" t="s">
-        <v>90</v>
-      </c>
-      <c r="C78" t="s">
-        <v>14</v>
-      </c>
-      <c r="D78" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <v>2</v>
-      </c>
-      <c r="B79" t="s">
-        <v>113</v>
-      </c>
-      <c r="C79" t="s">
-        <v>14</v>
-      </c>
-      <c r="D79" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>2</v>
-      </c>
-      <c r="B80" t="s">
-        <v>114</v>
-      </c>
-      <c r="C80" t="s">
-        <v>14</v>
-      </c>
-      <c r="D80" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>1</v>
-      </c>
-      <c r="B81" t="s">
-        <v>92</v>
-      </c>
-      <c r="C81" t="s">
-        <v>14</v>
-      </c>
-      <c r="D81" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82">
-        <v>1</v>
-      </c>
-      <c r="B82" t="s">
-        <v>115</v>
-      </c>
-      <c r="C82" t="s">
-        <v>14</v>
-      </c>
-      <c r="D82" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>1</v>
-      </c>
-      <c r="B83" t="s">
-        <v>93</v>
-      </c>
-      <c r="C83" t="s">
-        <v>14</v>
-      </c>
-      <c r="D83" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>1</v>
-      </c>
-      <c r="B84" t="s">
-        <v>94</v>
-      </c>
-      <c r="C84" t="s">
-        <v>14</v>
-      </c>
-      <c r="D84" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>1</v>
-      </c>
-      <c r="B85" t="s">
-        <v>95</v>
-      </c>
-      <c r="C85" t="s">
-        <v>14</v>
-      </c>
-      <c r="D85" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <v>1</v>
-      </c>
-      <c r="B86" t="s">
+        <v>147</v>
+      </c>
+      <c r="E62" t="s">
         <v>116</v>
       </c>
-      <c r="C86" t="s">
-        <v>14</v>
-      </c>
-      <c r="D86" t="s">
-        <v>91</v>
-      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B63"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B64"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B67"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B69"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B72"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B73"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B74"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B75"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B76"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B77"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B78"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B79"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B80"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B81"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B82"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B83"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B84"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B85"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B86"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2834,4 +2808,1229 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E05F322-5E86-4645-A92E-3EBDD0F8C4B3}">
+  <dimension ref="A1:D86"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11" style="2"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="37.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s">
+        <v>129</v>
+      </c>
+      <c r="D28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" t="s">
+        <v>129</v>
+      </c>
+      <c r="D29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>129</v>
+      </c>
+      <c r="D32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" t="s">
+        <v>129</v>
+      </c>
+      <c r="D36" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>131</v>
+      </c>
+      <c r="C37" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" t="s">
+        <v>129</v>
+      </c>
+      <c r="D39" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" t="s">
+        <v>129</v>
+      </c>
+      <c r="D40" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>4</v>
+      </c>
+      <c r="B42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" t="s">
+        <v>129</v>
+      </c>
+      <c r="D43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="B46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" t="s">
+        <v>129</v>
+      </c>
+      <c r="D46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>3</v>
+      </c>
+      <c r="B55" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>3</v>
+      </c>
+      <c r="B56" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>4</v>
+      </c>
+      <c r="B57" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>4</v>
+      </c>
+      <c r="B58" t="s">
+        <v>79</v>
+      </c>
+      <c r="C58" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>4</v>
+      </c>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>4</v>
+      </c>
+      <c r="B60" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>4</v>
+      </c>
+      <c r="B61" t="s">
+        <v>108</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>4</v>
+      </c>
+      <c r="B62" t="s">
+        <v>109</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" t="s">
+        <v>25</v>
+      </c>
+      <c r="D63" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
+        <v>130</v>
+      </c>
+      <c r="C64" t="s">
+        <v>25</v>
+      </c>
+      <c r="D64" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65" t="s">
+        <v>80</v>
+      </c>
+      <c r="C65" t="s">
+        <v>25</v>
+      </c>
+      <c r="D65" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66" t="s">
+        <v>63</v>
+      </c>
+      <c r="C66" t="s">
+        <v>25</v>
+      </c>
+      <c r="D66" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>2</v>
+      </c>
+      <c r="B67" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" t="s">
+        <v>25</v>
+      </c>
+      <c r="D67" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>2</v>
+      </c>
+      <c r="B68" t="s">
+        <v>62</v>
+      </c>
+      <c r="C68" t="s">
+        <v>25</v>
+      </c>
+      <c r="D68" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>2</v>
+      </c>
+      <c r="B69" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69" t="s">
+        <v>25</v>
+      </c>
+      <c r="D69" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>2</v>
+      </c>
+      <c r="B70" t="s">
+        <v>59</v>
+      </c>
+      <c r="C70" t="s">
+        <v>25</v>
+      </c>
+      <c r="D70" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>3</v>
+      </c>
+      <c r="B71" t="s">
+        <v>49</v>
+      </c>
+      <c r="C71" t="s">
+        <v>25</v>
+      </c>
+      <c r="D71" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>3</v>
+      </c>
+      <c r="B72" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72" t="s">
+        <v>25</v>
+      </c>
+      <c r="D72" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>3</v>
+      </c>
+      <c r="B73" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" t="s">
+        <v>25</v>
+      </c>
+      <c r="D73" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>3</v>
+      </c>
+      <c r="B74" t="s">
+        <v>86</v>
+      </c>
+      <c r="C74" t="s">
+        <v>25</v>
+      </c>
+      <c r="D74" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>2</v>
+      </c>
+      <c r="B75" t="s">
+        <v>87</v>
+      </c>
+      <c r="C75" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>2</v>
+      </c>
+      <c r="B76" t="s">
+        <v>88</v>
+      </c>
+      <c r="C76" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>2</v>
+      </c>
+      <c r="B77" t="s">
+        <v>89</v>
+      </c>
+      <c r="C77" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>2</v>
+      </c>
+      <c r="B78" t="s">
+        <v>90</v>
+      </c>
+      <c r="C78" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>2</v>
+      </c>
+      <c r="B79" t="s">
+        <v>113</v>
+      </c>
+      <c r="C79" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>2</v>
+      </c>
+      <c r="B80" t="s">
+        <v>114</v>
+      </c>
+      <c r="C80" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>1</v>
+      </c>
+      <c r="B81" t="s">
+        <v>92</v>
+      </c>
+      <c r="C81" t="s">
+        <v>14</v>
+      </c>
+      <c r="D81" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>1</v>
+      </c>
+      <c r="B82" t="s">
+        <v>115</v>
+      </c>
+      <c r="C82" t="s">
+        <v>14</v>
+      </c>
+      <c r="D82" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>1</v>
+      </c>
+      <c r="B83" t="s">
+        <v>93</v>
+      </c>
+      <c r="C83" t="s">
+        <v>14</v>
+      </c>
+      <c r="D83" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>1</v>
+      </c>
+      <c r="B84" t="s">
+        <v>94</v>
+      </c>
+      <c r="C84" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>1</v>
+      </c>
+      <c r="B85" t="s">
+        <v>95</v>
+      </c>
+      <c r="C85" t="s">
+        <v>14</v>
+      </c>
+      <c r="D85" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>1</v>
+      </c>
+      <c r="B86" t="s">
+        <v>116</v>
+      </c>
+      <c r="C86" t="s">
+        <v>14</v>
+      </c>
+      <c r="D86" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>